<commit_message>
experimental exec with 32 threads
</commit_message>
<xml_diff>
--- a/src/c++ backend/esp32-BasicMathExample/evaluation-2019-11-11.xlsx
+++ b/src/c++ backend/esp32-BasicMathExample/evaluation-2019-11-11.xlsx
@@ -1,74 +1,90 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720"/>
   </bookViews>
   <sheets>
-    <sheet name="8 threads" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="16 threads" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="8 threads" sheetId="1" r:id="rId1"/>
+    <sheet name="16 threads" sheetId="2" r:id="rId2"/>
+    <sheet name="32 threads" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
   <si>
-    <t xml:space="preserve">number of threads</t>
+    <t>number of threads</t>
   </si>
   <si>
-    <t xml:space="preserve">total speedup</t>
+    <t>total speedup</t>
   </si>
   <si>
-    <t xml:space="preserve">execution time (ms)</t>
+    <t>execution time (ms)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <b/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="12"/>
       <color theme="1"/>
-      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
-      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -97,26 +113,32 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="1" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="2" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="3" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="4" fillId="0" borderId="1" numFmtId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -125,16 +147,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="c14">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
       <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
@@ -146,6 +173,7 @@
       <c:tx>
         <c:rich>
           <a:bodyPr/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0">
@@ -158,10 +186,9 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr/>
+              <a:rPr lang="en-US"/>
               <a:t>Total speedup in dependence of </a:t>
             </a:r>
-            <a:endParaRPr/>
           </a:p>
           <a:p>
             <a:pPr>
@@ -175,41 +202,22 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr/>
+              <a:rPr lang="en-US"/>
               <a:t>used amount of threads</a:t>
             </a:r>
-            <a:endParaRPr/>
           </a:p>
         </c:rich>
       </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
-      <c:spPr bwMode="auto">
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+      <c:spPr>
         <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="true" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr/>
-        </a:p>
-      </c:txPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -218,37 +226,37 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:spPr bwMode="auto"/>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f xml:space="preserve">'8 threads'!$C$3:$C$10</c:f>
+              <c:f>'8 threads'!$C$3:$C$10</c:f>
               <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1" formatCode="0.00">
+                <c:pt idx="1">
                   <c:v>1.6</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0.00">
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="0.00">
-                  <c:v>2.18</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="0.00">
+                <c:pt idx="3">
+                  <c:v>2.1800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>2.5</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="0.00">
-                  <c:v>2.53</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="0.00">
+                <c:pt idx="5">
+                  <c:v>2.5299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>2.8</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="0.00">
+                <c:pt idx="7">
                   <c:v>2.87</c:v>
                 </c:pt>
               </c:numCache>
@@ -256,13 +264,21 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1005"/>
-        <c:axId val="1006"/>
+        <c:axId val="256704896"/>
+        <c:axId val="256706816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1005"/>
+        <c:axId val="256704896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -272,37 +288,25 @@
           <c:tx>
             <c:rich>
               <a:bodyPr/>
+              <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr/>
+                  <a:rPr lang="en-US"/>
                   <a:t>number of threads</a:t>
                 </a:r>
-                <a:endParaRPr/>
               </a:p>
             </c:rich>
           </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
-          <c:txPr>
-            <a:bodyPr/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr/>
-              </a:pPr>
-              <a:endParaRPr/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr bwMode="auto">
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
+        <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
@@ -315,7 +319,8 @@
           </a:ln>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="true" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0">
@@ -327,10 +332,10 @@
                 </a:solidFill>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1006"/>
+        <c:crossAx val="256706816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -339,17 +344,14 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1006"/>
+        <c:axId val="256706816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
+          <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -365,57 +367,47 @@
           <c:tx>
             <c:rich>
               <a:bodyPr/>
+              <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr/>
+                  <a:rPr lang="en-US"/>
                   <a:t>Speedup S = T</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr baseline="-25000"/>
+                  <a:rPr lang="en-US" baseline="-25000"/>
                   <a:t>1</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr/>
+                  <a:rPr lang="en-US"/>
                   <a:t> / T</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr baseline="-25000"/>
+                  <a:rPr lang="en-US" baseline="-25000"/>
                   <a:t>P</a:t>
                 </a:r>
-                <a:endParaRPr/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
-          <c:txPr>
-            <a:bodyPr/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr/>
-              </a:pPr>
-              <a:endParaRPr/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr bwMode="auto">
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
+        <c:spPr>
           <a:noFill/>
           <a:ln>
             <a:noFill/>
           </a:ln>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="true" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0">
@@ -427,17 +419,14 @@
                 </a:solidFill>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1005"/>
+        <c:crossAx val="256704896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:spPr bwMode="auto">
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+      <c:spPr>
         <a:noFill/>
         <a:ln>
           <a:noFill/>
@@ -448,14 +437,7 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:spPr bwMode="auto">
-    <a:xfrm>
-      <a:off x="207306" y="2382816"/>
-      <a:ext cx="5488641" cy="3341706"/>
-    </a:xfrm>
-    <a:prstGeom prst="rect">
-      <a:avLst/>
-    </a:prstGeom>
+  <c:spPr>
     <a:solidFill>
       <a:schemeClr val="bg1"/>
     </a:solidFill>
@@ -471,28 +453,29 @@
   </c:spPr>
   <c:txPr>
     <a:bodyPr/>
+    <a:lstStyle/>
     <a:p>
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins l="0.69999999999999996" r="0.69999999999999996" t="0.75" b="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="c14">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
       <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
@@ -504,6 +487,7 @@
       <c:tx>
         <c:rich>
           <a:bodyPr/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0">
@@ -516,10 +500,9 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr/>
+              <a:rPr lang="en-US"/>
               <a:t>Total speedup in dependence of </a:t>
             </a:r>
-            <a:endParaRPr/>
           </a:p>
           <a:p>
             <a:pPr>
@@ -533,41 +516,22 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr/>
+              <a:rPr lang="en-US"/>
               <a:t>used amount of threads</a:t>
             </a:r>
-            <a:endParaRPr/>
           </a:p>
         </c:rich>
       </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
-      <c:spPr bwMode="auto">
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+      <c:spPr>
         <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="true" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr/>
-        </a:p>
-      </c:txPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -576,61 +540,61 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:spPr bwMode="auto"/>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f xml:space="preserve">'16 threads'!$C$3:$C$18</c:f>
+              <c:f>'16 threads'!$C$3:$C$18</c:f>
               <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1" formatCode="0.00">
+                <c:pt idx="1">
                   <c:v>1.6</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0.00">
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="0.00">
-                  <c:v>2.18</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="0.00">
-                  <c:v>2.22</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="0.00">
+                <c:pt idx="3">
+                  <c:v>2.1800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>2.52</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="0.00">
+                <c:pt idx="6">
                   <c:v>2.54</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="0.00">
+                <c:pt idx="7">
                   <c:v>2.58</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="0.00">
+                <c:pt idx="8">
                   <c:v>2.61</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="0.00">
+                <c:pt idx="9">
                   <c:v>3.07</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="0.00">
+                <c:pt idx="10">
                   <c:v>2.7</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="0.00">
+                <c:pt idx="11">
                   <c:v>3.21</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="0.00">
+                <c:pt idx="12">
                   <c:v>3.18</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="0.00">
+                <c:pt idx="13">
                   <c:v>3.09</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="0.00">
+                <c:pt idx="14">
                   <c:v>3.1</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="0.00">
+                <c:pt idx="15">
                   <c:v>3.35</c:v>
                 </c:pt>
               </c:numCache>
@@ -638,13 +602,21 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1007"/>
-        <c:axId val="1008"/>
+        <c:axId val="256748160"/>
+        <c:axId val="256762624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1007"/>
+        <c:axId val="256748160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -654,37 +626,25 @@
           <c:tx>
             <c:rich>
               <a:bodyPr/>
+              <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr/>
+                  <a:rPr lang="en-US"/>
                   <a:t>number of threads</a:t>
                 </a:r>
-                <a:endParaRPr/>
               </a:p>
             </c:rich>
           </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
-          <c:txPr>
-            <a:bodyPr/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr/>
-              </a:pPr>
-              <a:endParaRPr/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr bwMode="auto">
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
+        <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
@@ -697,7 +657,8 @@
           </a:ln>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="true" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0">
@@ -709,10 +670,10 @@
                 </a:solidFill>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1008"/>
+        <c:crossAx val="256762624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -721,17 +682,14 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1008"/>
+        <c:axId val="256762624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
+          <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -747,57 +705,47 @@
           <c:tx>
             <c:rich>
               <a:bodyPr/>
+              <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr/>
+                  <a:rPr lang="en-US"/>
                   <a:t>Speedup S = T</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr baseline="-25000"/>
+                  <a:rPr lang="en-US" baseline="-25000"/>
                   <a:t>1</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr/>
+                  <a:rPr lang="en-US"/>
                   <a:t> / T</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr baseline="-25000"/>
+                  <a:rPr lang="en-US" baseline="-25000"/>
                   <a:t>P</a:t>
                 </a:r>
-                <a:endParaRPr/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
-          <c:txPr>
-            <a:bodyPr/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr/>
-              </a:pPr>
-              <a:endParaRPr/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr bwMode="auto">
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
+        <c:spPr>
           <a:noFill/>
           <a:ln>
             <a:noFill/>
           </a:ln>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="true" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0">
@@ -809,17 +757,14 @@
                 </a:solidFill>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1007"/>
+        <c:crossAx val="256748160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:spPr bwMode="auto">
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+      <c:spPr>
         <a:noFill/>
         <a:ln>
           <a:noFill/>
@@ -830,14 +775,7 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:spPr bwMode="auto">
-    <a:xfrm>
-      <a:off x="209549" y="3829048"/>
-      <a:ext cx="5488640" cy="3341706"/>
-    </a:xfrm>
-    <a:prstGeom prst="rect">
-      <a:avLst/>
-    </a:prstGeom>
+  <c:spPr>
     <a:solidFill>
       <a:schemeClr val="bg1"/>
     </a:solidFill>
@@ -851,23 +789,325 @@
   </c:spPr>
   <c:txPr>
     <a:bodyPr/>
+    <a:lstStyle/>
     <a:p>
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins l="0.69999999999999996" r="0.69999999999999996" t="0.75" b="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Total speedup in dependence of </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>used amount of threads</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.8681145545286555E-2"/>
+          <c:y val="0.13268733916403772"/>
+          <c:w val="0.80957860266891313"/>
+          <c:h val="0.77809976998624786"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>speedup</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'32 threads'!$C$3:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5995352735029713</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0002381746296383</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1808974758491741</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4991667658612071</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5244078393651557</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.7966033966033965</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.7542306178669813</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.9946512623020967</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.9198943049857449</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.1341244961934618</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.0452534629052144</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.2370490286771507</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.1425684777727887</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.316038853352286</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.2194280456950088</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.3806456807020369</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.284395776300352</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.4297966184758639</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.3350011913271382</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.4683241100189974</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.3798293625241467</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.5036295369211516</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.4177926094741982</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.5366798618714732</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="48215552"/>
+        <c:axId val="48217472"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="48215552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>number of threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="48217472"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="48217472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Speedup S = T</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" baseline="-25000">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>1</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t> / T</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" baseline="-25000">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>P</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="48215552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -881,16 +1121,16 @@
       <xdr:row>31</xdr:row>
       <xdr:rowOff>85723</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="" hidden="0"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="207306" y="2382816"/>
-        <a:ext cx="5488641" cy="3341706"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -904,30 +1144,30 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>209549</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>180973</xdr:rowOff>
+      <xdr:colOff>190499</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>190498</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>173690</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>84155</xdr:rowOff>
+      <xdr:colOff>154640</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>93680</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="" hidden="0"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="209549" y="3829048"/>
-        <a:ext cx="5488640" cy="3341706"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -940,291 +1180,43 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Angsana New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Cordia New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>63873</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57709</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>444874</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>113178</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1427,25 +1419,25 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="3.140625"/>
-    <col customWidth="1" min="2" max="2" width="20.8515625"/>
-    <col customWidth="1" min="3" max="3" width="18.8515625"/>
-    <col customWidth="1" min="4" max="4" width="23.140625"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row ht="16.5" r="2">
+    <row r="2" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1456,7 +1448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row ht="14.25" r="3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
         <v>1</v>
       </c>
@@ -1467,18 +1459,18 @@
         <v>41979</v>
       </c>
     </row>
-    <row ht="14.25" r="4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>2</v>
       </c>
       <c r="C4" s="3">
-        <v>1.6000000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="D4" s="2">
         <v>26245</v>
       </c>
     </row>
-    <row ht="14.25" r="5">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>3</v>
       </c>
@@ -1489,7 +1481,7 @@
         <v>20988</v>
       </c>
     </row>
-    <row ht="14.25" r="6">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>4</v>
       </c>
@@ -1500,7 +1492,7 @@
         <v>19245</v>
       </c>
     </row>
-    <row ht="14.25" r="7">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>5</v>
       </c>
@@ -1511,7 +1503,7 @@
         <v>16792</v>
       </c>
     </row>
-    <row ht="14.25" r="8">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>6</v>
       </c>
@@ -1522,30 +1514,30 @@
         <v>16621</v>
       </c>
     </row>
-    <row ht="14.25" r="9">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>7</v>
       </c>
       <c r="C9" s="3">
-        <v>2.7999999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="D9" s="2">
         <v>15001</v>
       </c>
     </row>
-    <row ht="14.25" r="10">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>8</v>
       </c>
       <c r="C10" s="3">
-        <v>2.8700000000000001</v>
+        <v>2.87</v>
       </c>
       <c r="D10" s="2">
         <v>14605</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="0" gridLines="0" gridLinesSet="0"/>
+  <printOptions gridLines="1" gridLinesSet="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId1"/>
@@ -1553,21 +1545,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="3.140625"/>
-    <col customWidth="1" min="2" max="2" width="22.7109375"/>
-    <col customWidth="1" min="3" max="3" width="17.140625"/>
-    <col customWidth="1" min="4" max="4" width="21.57421875"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row ht="16.5" r="2">
+    <row r="2" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1578,7 +1571,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
         <v>1</v>
       </c>
@@ -1589,18 +1582,18 @@
         <v>41979</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="5">
         <v>2</v>
       </c>
       <c r="C4" s="6">
-        <v>1.6000000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="D4" s="5">
         <v>26245</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
         <v>3</v>
       </c>
@@ -1611,7 +1604,7 @@
         <v>20988</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="5">
         <v>4</v>
       </c>
@@ -1622,7 +1615,7 @@
         <v>19246</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
         <v>5</v>
       </c>
@@ -1633,7 +1626,7 @@
         <v>18895</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
         <v>6</v>
       </c>
@@ -1644,7 +1637,7 @@
         <v>16629</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>7</v>
       </c>
@@ -1655,51 +1648,51 @@
         <v>16502</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>8</v>
       </c>
       <c r="C10" s="6">
-        <v>2.5800000000000001</v>
+        <v>2.58</v>
       </c>
       <c r="D10" s="5">
         <v>16284</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
         <v>9</v>
       </c>
       <c r="C11" s="6">
-        <v>2.6099999999999999</v>
+        <v>2.61</v>
       </c>
       <c r="D11" s="5">
         <v>16083</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
         <v>10</v>
       </c>
       <c r="C12" s="6">
-        <v>3.0699999999999998</v>
+        <v>3.07</v>
       </c>
       <c r="D12" s="5">
         <v>13695</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
         <v>11</v>
       </c>
       <c r="C13" s="6">
-        <v>2.7000000000000002</v>
+        <v>2.7</v>
       </c>
       <c r="D13" s="5">
         <v>15531</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>12</v>
       </c>
@@ -1710,54 +1703,437 @@
         <v>13069</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="5">
         <v>13</v>
       </c>
       <c r="C15" s="6">
-        <v>3.1800000000000002</v>
+        <v>3.18</v>
       </c>
       <c r="D15" s="5">
         <v>13184</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="5">
         <v>14</v>
       </c>
       <c r="C16" s="6">
-        <v>3.0899999999999999</v>
+        <v>3.09</v>
       </c>
       <c r="D16" s="5">
         <v>13575</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="5">
         <v>15</v>
       </c>
       <c r="C17" s="6">
-        <v>3.1000000000000001</v>
+        <v>3.1</v>
       </c>
       <c r="D17" s="5">
         <v>13559</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="5">
         <v>16</v>
       </c>
       <c r="C18" s="6">
-        <v>3.3500000000000001</v>
+        <v>3.35</v>
       </c>
       <c r="D18" s="5">
         <v>12528</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="0" gridLines="0" gridLinesSet="0"/>
+  <printOptions gridLines="1" gridLinesSet="0"/>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D34"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O42" sqref="O42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
+        <v>41991</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6">
+        <f>$D$3/D4</f>
+        <v>1.5995352735029713</v>
+      </c>
+      <c r="D4" s="5">
+        <v>26252</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="6">
+        <f>$D$3/D5</f>
+        <v>2.0002381746296383</v>
+      </c>
+      <c r="D5" s="5">
+        <v>20993</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="5">
+        <v>4</v>
+      </c>
+      <c r="C6" s="6">
+        <f>$D$3/D6</f>
+        <v>2.1808974758491741</v>
+      </c>
+      <c r="D6" s="5">
+        <v>19254</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="5">
+        <v>5</v>
+      </c>
+      <c r="C7" s="6">
+        <f t="shared" ref="C7:C27" si="0">$D$3/D7</f>
+        <v>2.4991667658612071</v>
+      </c>
+      <c r="D7" s="5">
+        <v>16802</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="5">
+        <v>6</v>
+      </c>
+      <c r="C8" s="6">
+        <f t="shared" si="0"/>
+        <v>2.5244078393651557</v>
+      </c>
+      <c r="D8" s="5">
+        <v>16634</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="5">
+        <v>7</v>
+      </c>
+      <c r="C9" s="6">
+        <f t="shared" si="0"/>
+        <v>2.7966033966033965</v>
+      </c>
+      <c r="D9" s="5">
+        <v>15015</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="5">
+        <v>8</v>
+      </c>
+      <c r="C10" s="6">
+        <f t="shared" si="0"/>
+        <v>2.7542306178669813</v>
+      </c>
+      <c r="D10" s="5">
+        <v>15246</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="5">
+        <v>9</v>
+      </c>
+      <c r="C11" s="6">
+        <f t="shared" si="0"/>
+        <v>2.9946512623020967</v>
+      </c>
+      <c r="D11" s="5">
+        <v>14022</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="5">
+        <v>10</v>
+      </c>
+      <c r="C12" s="6">
+        <f t="shared" si="0"/>
+        <v>2.9198943049857449</v>
+      </c>
+      <c r="D12" s="5">
+        <v>14381</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="5">
+        <v>11</v>
+      </c>
+      <c r="C13" s="6">
+        <f t="shared" si="0"/>
+        <v>3.1341244961934618</v>
+      </c>
+      <c r="D13" s="5">
+        <v>13398</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="5">
+        <v>12</v>
+      </c>
+      <c r="C14" s="6">
+        <f t="shared" si="0"/>
+        <v>3.0452534629052144</v>
+      </c>
+      <c r="D14" s="5">
+        <v>13789</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="5">
+        <v>13</v>
+      </c>
+      <c r="C15" s="6">
+        <f t="shared" si="0"/>
+        <v>3.2370490286771507</v>
+      </c>
+      <c r="D15" s="5">
+        <v>12972</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="5">
+        <v>14</v>
+      </c>
+      <c r="C16" s="6">
+        <f t="shared" si="0"/>
+        <v>3.1425684777727887</v>
+      </c>
+      <c r="D16" s="5">
+        <v>13362</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="5">
+        <v>15</v>
+      </c>
+      <c r="C17" s="6">
+        <f t="shared" si="0"/>
+        <v>3.316038853352286</v>
+      </c>
+      <c r="D17" s="5">
+        <v>12663</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="5">
+        <v>16</v>
+      </c>
+      <c r="C18" s="6">
+        <f t="shared" si="0"/>
+        <v>3.2194280456950088</v>
+      </c>
+      <c r="D18" s="5">
+        <v>13043</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="5">
+        <v>17</v>
+      </c>
+      <c r="C19" s="6">
+        <f t="shared" si="0"/>
+        <v>3.3806456807020369</v>
+      </c>
+      <c r="D19" s="5">
+        <v>12421</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="5">
+        <v>18</v>
+      </c>
+      <c r="C20" s="6">
+        <f t="shared" si="0"/>
+        <v>3.284395776300352</v>
+      </c>
+      <c r="D20" s="5">
+        <v>12785</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="5">
+        <v>19</v>
+      </c>
+      <c r="C21" s="6">
+        <f t="shared" si="0"/>
+        <v>3.4297966184758639</v>
+      </c>
+      <c r="D21" s="5">
+        <v>12243</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="5">
+        <v>20</v>
+      </c>
+      <c r="C22" s="6">
+        <f t="shared" si="0"/>
+        <v>3.3350011913271382</v>
+      </c>
+      <c r="D22" s="5">
+        <v>12591</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="5">
+        <v>21</v>
+      </c>
+      <c r="C23" s="6">
+        <f t="shared" si="0"/>
+        <v>3.4683241100189974</v>
+      </c>
+      <c r="D23" s="5">
+        <v>12107</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="5">
+        <v>22</v>
+      </c>
+      <c r="C24" s="6">
+        <f t="shared" si="0"/>
+        <v>3.3798293625241467</v>
+      </c>
+      <c r="D24" s="5">
+        <v>12424</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="5">
+        <v>23</v>
+      </c>
+      <c r="C25" s="6">
+        <f t="shared" si="0"/>
+        <v>3.5036295369211516</v>
+      </c>
+      <c r="D25" s="5">
+        <v>11985</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="5">
+        <v>24</v>
+      </c>
+      <c r="C26" s="6">
+        <f t="shared" si="0"/>
+        <v>3.4177926094741982</v>
+      </c>
+      <c r="D26" s="5">
+        <v>12286</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="5">
+        <v>25</v>
+      </c>
+      <c r="C27" s="6">
+        <f t="shared" si="0"/>
+        <v>3.5366798618714732</v>
+      </c>
+      <c r="D27" s="5">
+        <v>11873</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="5">
+        <v>26</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="8"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="5">
+        <v>27</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="5">
+        <v>28</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="5">
+        <v>29</v>
+      </c>
+      <c r="C31" s="7"/>
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="5">
+        <v>30</v>
+      </c>
+      <c r="C32" s="7"/>
+      <c r="D32" s="8"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="5">
+        <v>31</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="5">
+        <v>32</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="8"/>
+    </row>
+  </sheetData>
+  <printOptions gridLines="1" gridLinesSet="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>